<commit_message>
Update nfl-analysis, add position option in url
</commit_message>
<xml_diff>
--- a/project-code/Player_Rank.xlsx
+++ b/project-code/Player_Rank.xlsx
@@ -358,7 +358,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D28"/>
+  <dimension ref="A1:D49"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -389,14 +389,14 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Bryce Love</t>
+          <t>Hakeem Butler</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>191.2</v>
+        <v>158</v>
       </c>
       <c r="D2" t="n">
-        <v>11.95</v>
+        <v>9.875</v>
       </c>
     </row>
     <row r="3">
@@ -405,14 +405,14 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Karan Higdon</t>
+          <t>J.J. Arcega-Whiteside</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>174</v>
+        <v>135.16</v>
       </c>
       <c r="D3" t="n">
-        <v>10.875</v>
+        <v>8.4475</v>
       </c>
     </row>
     <row r="4">
@@ -421,14 +421,14 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Darrell Henderson</t>
+          <t>Darius Slayton</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>174</v>
+        <v>95.8</v>
       </c>
       <c r="D4" t="n">
-        <v>10.875</v>
+        <v>5.9875</v>
       </c>
     </row>
     <row r="5">
@@ -437,14 +437,14 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Jordan Scarlett</t>
+          <t>Mecole Hardman</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>125</v>
+        <v>95.05</v>
       </c>
       <c r="D5" t="n">
-        <v>7.8125</v>
+        <v>5.940625</v>
       </c>
     </row>
     <row r="6">
@@ -453,14 +453,14 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Dexter Williams</t>
+          <t>Jamal Custis</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>112.5454545454545</v>
+        <v>90.83333333333333</v>
       </c>
       <c r="D6" t="n">
-        <v>7.034090909090909</v>
+        <v>5.677083333333333</v>
       </c>
     </row>
     <row r="7">
@@ -469,14 +469,14 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Alexander Mattison</t>
+          <t>Damarkus Lodge</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>112.3076923076923</v>
+        <v>90.59999999999999</v>
       </c>
       <c r="D7" t="n">
-        <v>7.019230769230769</v>
+        <v>5.6625</v>
       </c>
     </row>
     <row r="8">
@@ -485,14 +485,14 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Lj Scott</t>
+          <t>Johnnie Dixon</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>104.4615384615385</v>
+        <v>89.90909090909091</v>
       </c>
       <c r="D8" t="n">
-        <v>6.528846153846154</v>
+        <v>5.619318181818182</v>
       </c>
     </row>
     <row r="9">
@@ -501,14 +501,14 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Qadree Ollison</t>
+          <t>Deebo Samuel</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>103.3571428571429</v>
+        <v>88.125</v>
       </c>
       <c r="D9" t="n">
-        <v>6.459821428571429</v>
+        <v>5.5078125</v>
       </c>
     </row>
     <row r="10">
@@ -517,14 +517,14 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Alex Barnes</t>
+          <t>Felton Davis</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>98.6875</v>
+        <v>85.47619047619048</v>
       </c>
       <c r="D10" t="n">
-        <v>6.16796875</v>
+        <v>5.342261904761905</v>
       </c>
     </row>
     <row r="11">
@@ -533,14 +533,14 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Damien Harris</t>
+          <t>Gary Jennings</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>83.33333333333333</v>
+        <v>83.5</v>
       </c>
       <c r="D11" t="n">
-        <v>5.208333333333333</v>
+        <v>5.21875</v>
       </c>
     </row>
     <row r="12">
@@ -549,14 +549,14 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>David Montgomery</t>
+          <t>Nyqwan Murray</t>
         </is>
       </c>
       <c r="C12" t="n">
-        <v>74.5</v>
+        <v>78.75</v>
       </c>
       <c r="D12" t="n">
-        <v>4.65625</v>
+        <v>4.921875</v>
       </c>
     </row>
     <row r="13">
@@ -565,14 +565,14 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>James Williams</t>
+          <t>D.K. Metcalf</t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>71</v>
+        <v>78.66666666666667</v>
       </c>
       <c r="D13" t="n">
-        <v>4.4375</v>
+        <v>4.916666666666667</v>
       </c>
     </row>
     <row r="14">
@@ -581,14 +581,14 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Tony Pollard</t>
+          <t>Riley Ridley</t>
         </is>
       </c>
       <c r="C14" t="n">
-        <v>62.57142857142857</v>
+        <v>78.16666666666667</v>
       </c>
       <c r="D14" t="n">
-        <v>3.910714285714286</v>
+        <v>4.885416666666667</v>
       </c>
     </row>
     <row r="15">
@@ -597,14 +597,14 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Josh Jacobs</t>
+          <t>Keesean Johnson</t>
         </is>
       </c>
       <c r="C15" t="n">
-        <v>55.5</v>
+        <v>78.16666666666667</v>
       </c>
       <c r="D15" t="n">
-        <v>3.46875</v>
+        <v>4.885416666666667</v>
       </c>
     </row>
     <row r="16">
@@ -613,14 +613,14 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Mike Weber</t>
+          <t>Terry McLaurin</t>
         </is>
       </c>
       <c r="C16" t="n">
-        <v>54.875</v>
+        <v>75.05263157894737</v>
       </c>
       <c r="D16" t="n">
-        <v>3.4296875</v>
+        <v>4.690789473684211</v>
       </c>
     </row>
     <row r="17">
@@ -629,14 +629,14 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Rodney Anderson</t>
+          <t>David Sills</t>
         </is>
       </c>
       <c r="C17" t="n">
-        <v>52.8</v>
+        <v>72.8</v>
       </c>
       <c r="D17" t="n">
-        <v>3.3</v>
+        <v>4.55</v>
       </c>
     </row>
     <row r="18">
@@ -645,14 +645,14 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Miles Sanders</t>
+          <t>Hunter Renfrow</t>
         </is>
       </c>
       <c r="C18" t="n">
-        <v>41.66666666666666</v>
+        <v>67.5</v>
       </c>
       <c r="D18" t="n">
-        <v>2.604166666666667</v>
+        <v>4.21875</v>
       </c>
     </row>
     <row r="19">
@@ -661,14 +661,14 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Travis Homer</t>
+          <t>Parris Campbell</t>
         </is>
       </c>
       <c r="C19" t="n">
-        <v>40.5</v>
+        <v>66.33333333333333</v>
       </c>
       <c r="D19" t="n">
-        <v>2.53125</v>
+        <v>4.145833333333333</v>
       </c>
     </row>
     <row r="20">
@@ -677,14 +677,14 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Trayveon Williams</t>
+          <t>Travis Fulgham</t>
         </is>
       </c>
       <c r="C20" t="n">
-        <v>38.4</v>
+        <v>49.81818181818182</v>
       </c>
       <c r="D20" t="n">
-        <v>2.4</v>
+        <v>3.113636363636364</v>
       </c>
     </row>
     <row r="21">
@@ -693,14 +693,14 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Myles Gaskin</t>
+          <t>Andy Isabella</t>
         </is>
       </c>
       <c r="C21" t="n">
-        <v>34</v>
+        <v>49.35294117647059</v>
       </c>
       <c r="D21" t="n">
-        <v>2.125</v>
+        <v>3.084558823529412</v>
       </c>
     </row>
     <row r="22">
@@ -709,14 +709,14 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Justice Hill</t>
+          <t>Miles Boykin</t>
         </is>
       </c>
       <c r="C22" t="n">
-        <v>23.25</v>
+        <v>48.4</v>
       </c>
       <c r="D22" t="n">
-        <v>1.453125</v>
+        <v>3.025</v>
       </c>
     </row>
     <row r="23">
@@ -725,14 +725,14 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Ryquell Armstead</t>
+          <t>Stanley Morgan</t>
         </is>
       </c>
       <c r="C23" t="n">
-        <v>18</v>
+        <v>47.42857142857143</v>
       </c>
       <c r="D23" t="n">
-        <v>1.125</v>
+        <v>2.964285714285714</v>
       </c>
     </row>
     <row r="24">
@@ -741,14 +741,14 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Elijah Holyfield</t>
+          <t>Emmanuel Butler</t>
         </is>
       </c>
       <c r="C24" t="n">
-        <v>10.33333333333333</v>
+        <v>46</v>
       </c>
       <c r="D24" t="n">
-        <v>0.6458333333333334</v>
+        <v>2.875</v>
       </c>
     </row>
     <row r="25">
@@ -757,14 +757,14 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Devin Singletary</t>
+          <t>Diontae Johnson</t>
         </is>
       </c>
       <c r="C25" t="n">
-        <v>8</v>
+        <v>40.07142857142857</v>
       </c>
       <c r="D25" t="n">
-        <v>0.5</v>
+        <v>2.504464285714286</v>
       </c>
     </row>
     <row r="26">
@@ -773,14 +773,14 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Nick Brossette</t>
+          <t>Jalen Hurd</t>
         </is>
       </c>
       <c r="C26" t="n">
-        <v>7.333333333333333</v>
+        <v>39.52941176470588</v>
       </c>
       <c r="D26" t="n">
-        <v>0.4583333333333333</v>
+        <v>2.470588235294118</v>
       </c>
     </row>
     <row r="27">
@@ -789,14 +789,14 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Benny Snell</t>
+          <t>Keelan Doss</t>
         </is>
       </c>
       <c r="C27" t="n">
-        <v>1.5</v>
+        <v>34</v>
       </c>
       <c r="D27" t="n">
-        <v>0.09375</v>
+        <v>2.125</v>
       </c>
     </row>
     <row r="28">
@@ -805,14 +805,350 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Jalin Moore</t>
+          <t>Ashton Dulin</t>
         </is>
       </c>
       <c r="C28" t="n">
+        <v>33.875</v>
+      </c>
+      <c r="D28" t="n">
+        <v>2.1171875</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="1" t="n">
+        <v>27</v>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>Tyre Brady</t>
+        </is>
+      </c>
+      <c r="C29" t="n">
+        <v>32</v>
+      </c>
+      <c r="D29" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="1" t="n">
+        <v>28</v>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>Antoine Wesley</t>
+        </is>
+      </c>
+      <c r="C30" t="n">
+        <v>28</v>
+      </c>
+      <c r="D30" t="n">
+        <v>1.75</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="1" t="n">
+        <v>29</v>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>Kelvin Harmon</t>
+        </is>
+      </c>
+      <c r="C31" t="n">
+        <v>28</v>
+      </c>
+      <c r="D31" t="n">
+        <v>1.75</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="1" t="n">
+        <v>30</v>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>Emanuel Hall</t>
+        </is>
+      </c>
+      <c r="C32" t="n">
+        <v>25.3</v>
+      </c>
+      <c r="D32" t="n">
+        <v>1.58125</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="1" t="n">
+        <v>31</v>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>N'Keal Harry</t>
+        </is>
+      </c>
+      <c r="C33" t="n">
+        <v>22.9</v>
+      </c>
+      <c r="D33" t="n">
+        <v>1.43125</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="1" t="n">
+        <v>32</v>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>Jakobi Meyers</t>
+        </is>
+      </c>
+      <c r="C34" t="n">
+        <v>21.33333333333333</v>
+      </c>
+      <c r="D34" t="n">
+        <v>1.333333333333333</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="1" t="n">
+        <v>33</v>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>A.J. Brown</t>
+        </is>
+      </c>
+      <c r="C35" t="n">
+        <v>20.25</v>
+      </c>
+      <c r="D35" t="n">
+        <v>1.265625</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="1" t="n">
+        <v>34</v>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>Terry Godwin</t>
+        </is>
+      </c>
+      <c r="C36" t="n">
+        <v>19.66666666666667</v>
+      </c>
+      <c r="D36" t="n">
+        <v>1.229166666666667</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="1" t="n">
+        <v>35</v>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>Bisi Johnson</t>
+        </is>
+      </c>
+      <c r="C37" t="n">
+        <v>16.8</v>
+      </c>
+      <c r="D37" t="n">
+        <v>1.05</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="1" t="n">
+        <v>36</v>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>Cody Thompson</t>
+        </is>
+      </c>
+      <c r="C38" t="n">
+        <v>13.28571428571429</v>
+      </c>
+      <c r="D38" t="n">
+        <v>0.8303571428571429</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="1" t="n">
+        <v>37</v>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>Lil'Jordan Humphrey</t>
+        </is>
+      </c>
+      <c r="C39" t="n">
+        <v>6</v>
+      </c>
+      <c r="D39" t="n">
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="1" t="n">
+        <v>38</v>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>Anthony Johnson</t>
+        </is>
+      </c>
+      <c r="C40" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="D40" t="n">
+        <v>0.28125</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="1" t="n">
+        <v>39</v>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>Alex Wesley</t>
+        </is>
+      </c>
+      <c r="C41" t="n">
+        <v>3.5</v>
+      </c>
+      <c r="D41" t="n">
+        <v>0.21875</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="1" t="n">
+        <v>40</v>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>Jaylen Smith</t>
+        </is>
+      </c>
+      <c r="C42" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="D42" t="n">
+        <v>0.15625</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="1" t="n">
+        <v>41</v>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>Jovon Durante</t>
+        </is>
+      </c>
+      <c r="C43" t="n">
         <v>1</v>
       </c>
-      <c r="D28" t="n">
+      <c r="D43" t="n">
         <v>0.0625</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="1" t="n">
+        <v>42</v>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>Ryan Davis</t>
+        </is>
+      </c>
+      <c r="C44" t="n">
+        <v>1</v>
+      </c>
+      <c r="D44" t="n">
+        <v>0.0625</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="1" t="n">
+        <v>43</v>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>Dillon Mitchell</t>
+        </is>
+      </c>
+      <c r="C45" t="n">
+        <v>1</v>
+      </c>
+      <c r="D45" t="n">
+        <v>0.0625</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="1" t="n">
+        <v>44</v>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>Marquise Brown</t>
+        </is>
+      </c>
+      <c r="C46" t="n">
+        <v>0</v>
+      </c>
+      <c r="D46" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="1" t="n">
+        <v>45</v>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>Jamarius Way</t>
+        </is>
+      </c>
+      <c r="C47" t="n">
+        <v>0</v>
+      </c>
+      <c r="D47" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="1" t="n">
+        <v>46</v>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>Greg Dortch</t>
+        </is>
+      </c>
+      <c r="C48" t="n">
+        <v>0</v>
+      </c>
+      <c r="D48" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="1" t="n">
+        <v>47</v>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>Jazz Ferguson</t>
+        </is>
+      </c>
+      <c r="C49" t="n">
+        <v>0</v>
+      </c>
+      <c r="D49" t="n">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>